<commit_message>
don't read past the end of valid data on Parameters With Distributions
</commit_message>
<xml_diff>
--- a/inst/extdata/SF-April13.xlsx
+++ b/inst/extdata/SF-April13.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lbalzer/Dropbox/LEMMA_shared/JS code branch/lemma-temp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Dropbox (UC Berkeley Biostat)/LEMMA_shared/JS code branch/LEMMA/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E69B94F3-2F89-1449-8D12-48D352944F45}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3647656-6C7B-8A46-874E-4955BB13161A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5280" yWindow="2140" windowWidth="23580" windowHeight="17440" xr2:uid="{50240998-A895-7F42-B834-945925070EED}"/>
+    <workbookView xWindow="5280" yWindow="2140" windowWidth="23580" windowHeight="17440" activeTab="3" xr2:uid="{50240998-A895-7F42-B834-945925070EED}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters with Distributions" sheetId="1" r:id="rId1"/>
@@ -744,8 +744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACF7E970-76F8-6942-B4A0-7B2C1D2884B8}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="B2" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1298,6 +1298,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <dataValidations count="5">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C21:G22" xr:uid="{4DE0DCAE-C019-834F-B9C1-56C11EC5B821}">
       <formula1>$A$27:$A$28</formula1>
@@ -1328,7 +1329,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1371,6 +1372,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <dataValidations count="2">
     <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{88106E44-DD25-724E-9428-A2C12A1073F6}">
       <formula1>0</formula1>
@@ -1390,7 +1392,7 @@
   <dimension ref="A1:D48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1732,6 +1734,7 @@
       <c r="A48" s="13"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <dataValidations count="2">
     <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A390" xr:uid="{140C1EC3-30A5-2448-BEAA-24AD135906D1}">
       <formula1>43831</formula1>
@@ -1750,8 +1753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99DD5F9C-4676-5749-AB11-9739EC646DB2}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1911,6 +1914,7 @@
       <c r="C17"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <dataValidations count="8">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{7D54BBB7-AF7C-3841-89CF-D6BEAE84ECD4}">
       <formula1>1</formula1>

</xml_diff>

<commit_message>
make min.obs.date.to.fit blank in SF_April13.xlsx
</commit_message>
<xml_diff>
--- a/inst/extdata/SF-April13.xlsx
+++ b/inst/extdata/SF-April13.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Dropbox (UC Berkeley Biostat)/LEMMA_shared/JS code branch/LEMMA/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8694CA3B-9E83-1543-BFA9-5D4853F5E4E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE48DA3-7692-D342-86AD-665064ED4F18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5280" yWindow="2140" windowWidth="23580" windowHeight="17440" xr2:uid="{50240998-A895-7F42-B834-945925070EED}"/>
+    <workbookView xWindow="5280" yWindow="2140" windowWidth="23580" windowHeight="17440" activeTab="3" xr2:uid="{50240998-A895-7F42-B834-945925070EED}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters with Distributions" sheetId="1" r:id="rId1"/>
@@ -744,7 +744,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACF7E970-76F8-6942-B4A0-7B2C1D2884B8}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView topLeftCell="B2" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1753,8 +1753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99DD5F9C-4676-5749-AB11-9739EC646DB2}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1842,9 +1842,7 @@
       <c r="A9" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="11">
-        <v>43906</v>
-      </c>
+      <c r="B9" s="11"/>
       <c r="C9" s="1" t="s">
         <v>67</v>
       </c>

</xml_diff>

<commit_message>
Add Projection Start Date to Excel input
</commit_message>
<xml_diff>
--- a/inst/extdata/SF-April13.xlsx
+++ b/inst/extdata/SF-April13.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Dropbox (UC Berkeley Biostat)/LEMMA_shared/JS code branch/LEMMA/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE48DA3-7692-D342-86AD-665064ED4F18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A4156AE-5F2F-5848-A24F-BE25972A6444}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5280" yWindow="2140" windowWidth="23580" windowHeight="17440" activeTab="3" xr2:uid="{50240998-A895-7F42-B834-945925070EED}"/>
+    <workbookView xWindow="5280" yWindow="2140" windowWidth="23580" windowHeight="17440" xr2:uid="{50240998-A895-7F42-B834-945925070EED}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters with Distributions" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="86">
   <si>
     <t>Number of Days from Infection to Becoming Infectious (Latent Period)</t>
   </si>
@@ -280,6 +280,12 @@
   </si>
   <si>
     <t>Priors</t>
+  </si>
+  <si>
+    <t>start.display.date</t>
+  </si>
+  <si>
+    <t>Projection Start Date</t>
   </si>
 </sst>
 </file>
@@ -744,8 +750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACF7E970-76F8-6942-B4A0-7B2C1D2884B8}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView topLeftCell="B2" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1326,10 +1332,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BCB5455-61A0-9A48-A110-20902745EBF4}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1362,12 +1368,23 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="6">
+        <v>43905</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C4" s="10">
         <v>43952</v>
       </c>
     </row>
@@ -1378,7 +1395,7 @@
       <formula1>0</formula1>
       <formula2>100000000</formula2>
     </dataValidation>
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{E9B6D3E5-D408-1D41-9CF1-E5EA3191C411}">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C4" xr:uid="{E9B6D3E5-D408-1D41-9CF1-E5EA3191C411}">
       <formula1>43831</formula1>
       <formula2>44561</formula2>
     </dataValidation>
@@ -1753,8 +1770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99DD5F9C-4676-5749-AB11-9739EC646DB2}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
return plots from PlotHist
</commit_message>
<xml_diff>
--- a/inst/extdata/SF-April13.xlsx
+++ b/inst/extdata/SF-April13.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Dropbox (UC Berkeley Biostat)/jsLEMMA/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92DD54CC-AD24-8E44-A0F6-5A1716D1C836}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1118D0A-A157-3143-B40C-F0C63906F134}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9660" yWindow="2040" windowWidth="23580" windowHeight="17440" xr2:uid="{50240998-A895-7F42-B834-945925070EED}"/>
   </bookViews>
@@ -1362,7 +1362,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1726,7 +1726,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>